<commit_message>
final plot in REplot
</commit_message>
<xml_diff>
--- a/matrix_detail.xlsx
+++ b/matrix_detail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenzh/Documents/GitHub/ColorectalCancerSimulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C836038-3075-6E45-8F6C-445C1E064BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA97A1D9-1AB1-D143-AD57-148CFC6310B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="11360" windowWidth="28040" windowHeight="17440" xr2:uid="{D3EA822C-3E36-7949-82D2-0163633F49A8}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{D3EA822C-3E36-7949-82D2-0163633F49A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -303,7 +303,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA9694C-CCD6-AF46-8530-0A136C039D0B}">
   <dimension ref="A1:AL33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="AJ2" sqref="AJ2"/>
+    <sheetView tabSelected="1" topLeftCell="AE3" zoomScale="133" workbookViewId="0">
+      <selection activeCell="AI10" sqref="AI10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2141,5 +2141,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>